<commit_message>
removed a duplicate column in blp data template file
</commit_message>
<xml_diff>
--- a/Template_BlpData.xlsx
+++ b/Template_BlpData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steven.zhang\AppData\Local\Programs\Git\git\risk_report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29F19FBA-BA36-4EEE-9BBE-5DC80802F030}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB87DCB5-B1B7-46BA-A620-B6FDD563C08E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2145" yWindow="915" windowWidth="21960" windowHeight="14850" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>ID</t>
   </si>
@@ -175,267 +175,195 @@
   <volType type="realTimeData">
     <main first="bloomberg.rtd">
       <tp t="s">
-        <v>#N/A Field Not Applicable</v>
+        <v>#N/A Connection</v>
+        <stp/>
+        <stp>##V3_BDPV12</stp>
+        <stp>XS2125922349 ISIN</stp>
+        <stp>CAPITAL_CONTINGENT_SECURITY</stp>
+        <stp>[Template_BlpData.xlsx]Sheet1!R4C8</stp>
+        <tr r="H4" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A Connection</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>XS2114413565 ISIN</stp>
         <stp>CAPITAL_CONTINGENT_SECURITY</stp>
-        <stp>[BlpData_Template.xlsx]Sheet1!R3C9</stp>
+        <stp>[Template_BlpData.xlsx]Sheet1!R3C8</stp>
+        <tr r="H3" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A Connection</v>
+        <stp/>
+        <stp>##V3_BDPV12</stp>
+        <stp>XS2125922349 ISIN</stp>
+        <stp>SFC_AUTHORIZED_FUND</stp>
+        <stp>[Template_BlpData.xlsx]Sheet1!R4C9</stp>
+        <tr r="I4" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A Connection</v>
+        <stp/>
+        <stp>##V3_BDPV12</stp>
+        <stp>XS2114413565 ISIN</stp>
+        <stp>SFC_AUTHORIZED_FUND</stp>
+        <stp>[Template_BlpData.xlsx]Sheet1!R3C9</stp>
         <tr r="I3" s="1"/>
       </tp>
       <tp t="s">
-        <v>Y</v>
-        <stp/>
-        <stp>##V3_BDPV12</stp>
-        <stp>XS2125922349 ISIN</stp>
-        <stp>CAPITAL_CONTINGENT_SECURITY</stp>
-        <stp>[BlpData_Template.xlsx]Sheet1!R4C9</stp>
-        <tr r="I4" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A Field Not Applicable</v>
+        <v>#N/A Connection</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>700 HK Equity</stp>
         <stp>SFC_AUTHORIZED_FUND</stp>
-        <stp>[BlpData_Template.xlsx]Sheet1!R2C10</stp>
-        <tr r="J2" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A Field Not Applicable</v>
-        <stp/>
-        <stp>##V3_BDPV12</stp>
-        <stp>XS2114413565 ISIN</stp>
-        <stp>SFC_AUTHORIZED_FUND</stp>
-        <stp>[BlpData_Template.xlsx]Sheet1!R3C10</stp>
-        <tr r="J3" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>CN</v>
+        <stp>[Template_BlpData.xlsx]Sheet1!R2C9</stp>
+        <tr r="I2" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A Connection</v>
+        <stp/>
+        <stp>##V3_BDPV12</stp>
+        <stp>700 HK Equity</stp>
+        <stp>CAPITAL_CONTINGENT_SECURITY</stp>
+        <stp>[Template_BlpData.xlsx]Sheet1!R2C8</stp>
+        <tr r="H2" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A Connection</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>700 HK Equity</stp>
         <stp>CNTRY_OF_RISK</stp>
-        <stp>[BlpData_Template.xlsx]Sheet1!R2C5</stp>
+        <stp>[Template_BlpData.xlsx]Sheet1!R2C5</stp>
         <tr r="E2" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A Field Not Applicable</v>
-        <stp/>
-        <stp>##V3_BDPV12</stp>
-        <stp>XS2125922349 ISIN</stp>
-        <stp>SFC_AUTHORIZED_FUND</stp>
-        <stp>[BlpData_Template.xlsx]Sheet1!R4C10</stp>
-        <tr r="J4" s="1"/>
       </tp>
     </main>
     <main first="bloomberg.rtd">
       <tp t="s">
-        <v>BB+</v>
-        <stp/>
-        <stp>##V3_BDPV12</stp>
-        <stp>XS2114413565 ISIN</stp>
-        <stp>RTG_SP</stp>
-        <stp>[BlpData_Template.xlsx]Sheet1!R3C11</stp>
-        <tr r="K3" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>BB+</v>
+        <v>#N/A Connection</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>XS2125922349 ISIN</stp>
-        <stp>RTG_SP</stp>
-        <stp>[BlpData_Template.xlsx]Sheet1!R4C11</stp>
-        <tr r="K4" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>Corp</v>
+        <stp>MARKET_SECTOR_DES</stp>
+        <stp>[Template_BlpData.xlsx]Sheet1!R4C3</stp>
+        <tr r="C4" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A Connection</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>XS2114413565 ISIN</stp>
         <stp>MARKET_SECTOR_DES</stp>
-        <stp>[BlpData_Template.xlsx]Sheet1!R3C6</stp>
-        <tr r="F3" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>Corp</v>
-        <stp/>
-        <stp>##V3_BDPV12</stp>
-        <stp>XS2114413565 ISIN</stp>
-        <stp>MARKET_SECTOR_DES</stp>
-        <stp>[BlpData_Template.xlsx]Sheet1!R3C3</stp>
+        <stp>[Template_BlpData.xlsx]Sheet1!R3C3</stp>
         <tr r="C3" s="1"/>
       </tp>
       <tp t="s">
-        <v>Corp</v>
-        <stp/>
-        <stp>##V3_BDPV12</stp>
-        <stp>XS2125922349 ISIN</stp>
-        <stp>MARKET_SECTOR_DES</stp>
-        <stp>[BlpData_Template.xlsx]Sheet1!R4C3</stp>
-        <tr r="C4" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>Corp</v>
-        <stp/>
-        <stp>##V3_BDPV12</stp>
-        <stp>XS2125922349 ISIN</stp>
-        <stp>MARKET_SECTOR_DES</stp>
-        <stp>[BlpData_Template.xlsx]Sheet1!R4C6</stp>
-        <tr r="F4" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>ACTV</v>
+        <v>#N/A Connection</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>XS2125922349 ISIN</stp>
         <stp>EXCH_MARKET_STATUS</stp>
-        <stp>[BlpData_Template.xlsx]Sheet1!R4C7</stp>
-        <tr r="G4" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>ACTV</v>
+        <stp>[Template_BlpData.xlsx]Sheet1!R4C6</stp>
+        <tr r="F4" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A Connection</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>XS2114413565 ISIN</stp>
         <stp>EXCH_MARKET_STATUS</stp>
-        <stp>[BlpData_Template.xlsx]Sheet1!R3C7</stp>
-        <tr r="G3" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>Communications</v>
+        <stp>[Template_BlpData.xlsx]Sheet1!R3C6</stp>
+        <tr r="F3" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A Connection</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>700 HK Equity</stp>
         <stp>INDUSTRY_SECTOR</stp>
-        <stp>[BlpData_Template.xlsx]Sheet1!R2C8</stp>
-        <tr r="H2" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>CN</v>
+        <stp>[Template_BlpData.xlsx]Sheet1!R2C7</stp>
+        <tr r="G2" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A Connection</v>
+        <stp/>
+        <stp>##V3_BDPV12</stp>
+        <stp>XS2114413565 ISIN</stp>
+        <stp>CNTRY_ISSUE_ISO</stp>
+        <stp>[Template_BlpData.xlsx]Sheet1!R3C4</stp>
+        <tr r="D3" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A Connection</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>XS2125922349 ISIN</stp>
         <stp>CNTRY_ISSUE_ISO</stp>
-        <stp>[BlpData_Template.xlsx]Sheet1!R4C4</stp>
+        <stp>[Template_BlpData.xlsx]Sheet1!R4C4</stp>
         <tr r="D4" s="1"/>
       </tp>
       <tp t="s">
-        <v>US</v>
-        <stp/>
-        <stp>##V3_BDPV12</stp>
-        <stp>XS2114413565 ISIN</stp>
-        <stp>CNTRY_ISSUE_ISO</stp>
-        <stp>[BlpData_Template.xlsx]Sheet1!R3C4</stp>
-        <tr r="D3" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>Ba1</v>
-        <stp/>
-        <stp>##V3_BDPV12</stp>
-        <stp>XS2125922349 ISIN</stp>
-        <stp>RTG_MOODY</stp>
-        <stp>[BlpData_Template.xlsx]Sheet1!R4C12</stp>
-        <tr r="L4" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>Ba1</v>
-        <stp/>
-        <stp>##V3_BDPV12</stp>
-        <stp>XS2114413565 ISIN</stp>
-        <stp>RTG_MOODY</stp>
-        <stp>[BlpData_Template.xlsx]Sheet1!R3C12</stp>
-        <tr r="L3" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>HK</v>
+        <v>#N/A Connection</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>700 HK Equity</stp>
         <stp>CNTRY_ISSUE_ISO</stp>
-        <stp>[BlpData_Template.xlsx]Sheet1!R2C4</stp>
+        <stp>[Template_BlpData.xlsx]Sheet1!R2C4</stp>
         <tr r="D2" s="1"/>
       </tp>
       <tp t="s">
-        <v>Financial</v>
+        <v>#N/A Connection</v>
+        <stp/>
+        <stp>##V3_BDPV12</stp>
+        <stp>XS2114413565 ISIN</stp>
+        <stp>INDUSTRY_SECTOR</stp>
+        <stp>[Template_BlpData.xlsx]Sheet1!R3C7</stp>
+        <tr r="G3" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A Connection</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>XS2125922349 ISIN</stp>
         <stp>INDUSTRY_SECTOR</stp>
-        <stp>[BlpData_Template.xlsx]Sheet1!R4C8</stp>
-        <tr r="H4" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>Communications</v>
-        <stp/>
-        <stp>##V3_BDPV12</stp>
-        <stp>XS2114413565 ISIN</stp>
-        <stp>INDUSTRY_SECTOR</stp>
-        <stp>[BlpData_Template.xlsx]Sheet1!R3C8</stp>
-        <tr r="H3" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>BBB</v>
-        <stp/>
-        <stp>##V3_BDPV12</stp>
-        <stp>XS2114413565 ISIN</stp>
-        <stp>RTG_FITCH</stp>
-        <stp>[BlpData_Template.xlsx]Sheet1!R3C13</stp>
-        <tr r="M3" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>Equity</v>
+        <stp>[Template_BlpData.xlsx]Sheet1!R4C7</stp>
+        <tr r="G4" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A Connection</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>700 HK Equity</stp>
         <stp>MARKET_SECTOR_DES</stp>
-        <stp>[BlpData_Template.xlsx]Sheet1!R2C3</stp>
+        <stp>[Template_BlpData.xlsx]Sheet1!R2C3</stp>
         <tr r="C2" s="1"/>
       </tp>
       <tp t="s">
-        <v>Equity</v>
-        <stp/>
-        <stp>##V3_BDPV12</stp>
-        <stp>700 HK Equity</stp>
-        <stp>MARKET_SECTOR_DES</stp>
-        <stp>[BlpData_Template.xlsx]Sheet1!R2C6</stp>
-        <tr r="F2" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>BB+</v>
-        <stp/>
-        <stp>##V3_BDPV12</stp>
-        <stp>XS2125922349 ISIN</stp>
-        <stp>RTG_FITCH</stp>
-        <stp>[BlpData_Template.xlsx]Sheet1!R4C13</stp>
-        <tr r="M4" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>CN</v>
+        <v>#N/A Connection</v>
+        <stp/>
+        <stp>##V3_BDPV12</stp>
+        <stp>XS2114413565 ISIN</stp>
+        <stp>CNTRY_OF_RISK</stp>
+        <stp>[Template_BlpData.xlsx]Sheet1!R3C5</stp>
+        <tr r="E3" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A Connection</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>XS2125922349 ISIN</stp>
         <stp>CNTRY_OF_RISK</stp>
-        <stp>[BlpData_Template.xlsx]Sheet1!R4C5</stp>
+        <stp>[Template_BlpData.xlsx]Sheet1!R4C5</stp>
         <tr r="E4" s="1"/>
       </tp>
       <tp t="s">
-        <v>US</v>
-        <stp/>
-        <stp>##V3_BDPV12</stp>
-        <stp>XS2114413565 ISIN</stp>
-        <stp>CNTRY_OF_RISK</stp>
-        <stp>[BlpData_Template.xlsx]Sheet1!R3C5</stp>
-        <tr r="E3" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>ACTV</v>
+        <v>#N/A Connection</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>700 HK Equity</stp>
         <stp>EXCH_MARKET_STATUS</stp>
-        <stp>[BlpData_Template.xlsx]Sheet1!R2C7</stp>
-        <tr r="G2" s="1"/>
+        <stp>[Template_BlpData.xlsx]Sheet1!R2C6</stp>
+        <tr r="F2" s="1"/>
       </tp>
     </main>
   </volType>
@@ -705,10 +633,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M4"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -718,17 +646,16 @@
     <col min="3" max="3" width="19.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.5703125" customWidth="1"/>
-    <col min="9" max="9" width="29.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="24.140625" customWidth="1"/>
-    <col min="11" max="11" width="11.140625" customWidth="1"/>
-    <col min="12" max="12" width="13" customWidth="1"/>
-    <col min="13" max="13" width="12.85546875" customWidth="1"/>
+    <col min="6" max="6" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.5703125" customWidth="1"/>
+    <col min="8" max="8" width="29.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.140625" customWidth="1"/>
+    <col min="10" max="10" width="11.140625" customWidth="1"/>
+    <col min="11" max="11" width="13" customWidth="1"/>
+    <col min="12" max="12" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -745,31 +672,28 @@
         <v>3</v>
       </c>
       <c r="F1" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="G1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="H1" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="I1" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="J1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="K1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="L1" t="s">
-        <v>14</v>
-      </c>
-      <c r="M1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -778,35 +702,35 @@
       </c>
       <c r="C2" t="str" cm="1">
         <f t="array" ref="C2">IF($B2="TICKER", _xll.BDP($A2,C$1), _xll.BDP($A2&amp;" "&amp;$B2, C$1))</f>
-        <v>Equity</v>
+        <v>#N/A Connection</v>
       </c>
       <c r="D2" t="str" cm="1">
         <f t="array" ref="D2">IF($B2="TICKER", _xll.BDP($A2,D$1), _xll.BDP($A2&amp;" "&amp;$B2, D$1))</f>
-        <v>HK</v>
+        <v>#N/A Connection</v>
       </c>
       <c r="E2" t="str" cm="1">
         <f t="array" ref="E2">IF($B2="TICKER", _xll.BDP($A2,E$1), _xll.BDP($A2&amp;" "&amp;$B2, E$1))</f>
-        <v>CN</v>
+        <v>#N/A Connection</v>
       </c>
       <c r="F2" t="str" cm="1">
         <f t="array" ref="F2">IF($B2="TICKER", _xll.BDP($A2,F$1), _xll.BDP($A2&amp;" "&amp;$B2, F$1))</f>
-        <v>Equity</v>
+        <v>#N/A Connection</v>
       </c>
       <c r="G2" t="str" cm="1">
         <f t="array" ref="G2">IF($B2="TICKER", _xll.BDP($A2,G$1), _xll.BDP($A2&amp;" "&amp;$B2, G$1))</f>
-        <v>ACTV</v>
+        <v>#N/A Connection</v>
       </c>
       <c r="H2" t="str" cm="1">
-        <f t="array" ref="H2">IF($B2="TICKER", _xll.BDP($A2,H$1), _xll.BDP($A2&amp;" "&amp;$B2, H$1))</f>
-        <v>Communications</v>
+        <f t="array" ref="H2">IF(C2="Equity", "N", IF($B2="TICKER", _xll.BDP($A2,H$1), _xll.BDP($A2&amp;" "&amp;$B2, H$1)))</f>
+        <v>#N/A Connection</v>
       </c>
       <c r="I2" t="str" cm="1">
-        <f t="array" ref="I2">IF(C2="Equity", "N", IF($B2="TICKER", _xll.BDP($A2,I$1), _xll.BDP($A2&amp;" "&amp;$B2, I$1)))</f>
-        <v>N</v>
+        <f t="array" ref="I2">IF($B2="TICKER", _xll.BDP($A2,I$1), _xll.BDP($A2&amp;" "&amp;$B2, I$1))</f>
+        <v>#N/A Connection</v>
       </c>
       <c r="J2" t="str" cm="1">
-        <f t="array" ref="J2">IF($B2="TICKER", _xll.BDP($A2,J$1), _xll.BDP($A2&amp;" "&amp;$B2, J$1))</f>
-        <v>#N/A Field Not Applicable</v>
+        <f t="array" ref="J2">IF(OR($C2="Corp", $C2="Govt"), IF($B2="TICKER", _xll.BDP($A2,J$1), _xll.BDP($A2&amp;" "&amp;$B2, J$1)), "#N/A")</f>
+        <v>#N/A</v>
       </c>
       <c r="K2" t="str" cm="1">
         <f t="array" ref="K2">IF(OR($C2="Corp", $C2="Govt"), IF($B2="TICKER", _xll.BDP($A2,K$1), _xll.BDP($A2&amp;" "&amp;$B2, K$1)), "#N/A")</f>
@@ -816,12 +740,8 @@
         <f t="array" ref="L2">IF(OR($C2="Corp", $C2="Govt"), IF($B2="TICKER", _xll.BDP($A2,L$1), _xll.BDP($A2&amp;" "&amp;$B2, L$1)), "#N/A")</f>
         <v>#N/A</v>
       </c>
-      <c r="M2" t="str" cm="1">
-        <f t="array" ref="M2">IF(OR($C2="Corp", $C2="Govt"), IF($B2="TICKER", _xll.BDP($A2,M$1), _xll.BDP($A2&amp;" "&amp;$B2, M$1)), "#N/A")</f>
-        <v>#N/A</v>
-      </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -830,50 +750,46 @@
       </c>
       <c r="C3" t="str" cm="1">
         <f t="array" ref="C3">IF($B3="TICKER", _xll.BDP($A3,C$1), _xll.BDP($A3&amp;" "&amp;$B3, C$1))</f>
-        <v>Corp</v>
+        <v>#N/A Connection</v>
       </c>
       <c r="D3" t="str" cm="1">
         <f t="array" ref="D3">IF($B3="TICKER", _xll.BDP($A3,D$1), _xll.BDP($A3&amp;" "&amp;$B3, D$1))</f>
-        <v>US</v>
+        <v>#N/A Connection</v>
       </c>
       <c r="E3" t="str" cm="1">
         <f t="array" ref="E3">IF($B3="TICKER", _xll.BDP($A3,E$1), _xll.BDP($A3&amp;" "&amp;$B3, E$1))</f>
-        <v>US</v>
+        <v>#N/A Connection</v>
       </c>
       <c r="F3" t="str" cm="1">
         <f t="array" ref="F3">IF($B3="TICKER", _xll.BDP($A3,F$1), _xll.BDP($A3&amp;" "&amp;$B3, F$1))</f>
-        <v>Corp</v>
+        <v>#N/A Connection</v>
       </c>
       <c r="G3" t="str" cm="1">
         <f t="array" ref="G3">IF($B3="TICKER", _xll.BDP($A3,G$1), _xll.BDP($A3&amp;" "&amp;$B3, G$1))</f>
-        <v>ACTV</v>
+        <v>#N/A Connection</v>
       </c>
       <c r="H3" t="str" cm="1">
-        <f t="array" ref="H3">IF($B3="TICKER", _xll.BDP($A3,H$1), _xll.BDP($A3&amp;" "&amp;$B3, H$1))</f>
-        <v>Communications</v>
+        <f t="array" ref="H3">IF(C3="Equity", "N", IF($B3="TICKER", _xll.BDP($A3,H$1), _xll.BDP($A3&amp;" "&amp;$B3, H$1)))</f>
+        <v>#N/A Connection</v>
       </c>
       <c r="I3" t="str" cm="1">
-        <f t="array" ref="I3">IF(C3="Equity", "N", IF($B3="TICKER", _xll.BDP($A3,I$1), _xll.BDP($A3&amp;" "&amp;$B3, I$1)))</f>
-        <v>#N/A Field Not Applicable</v>
+        <f t="array" ref="I3">IF($B3="TICKER", _xll.BDP($A3,I$1), _xll.BDP($A3&amp;" "&amp;$B3, I$1))</f>
+        <v>#N/A Connection</v>
       </c>
       <c r="J3" t="str" cm="1">
-        <f t="array" ref="J3">IF($B3="TICKER", _xll.BDP($A3,J$1), _xll.BDP($A3&amp;" "&amp;$B3, J$1))</f>
-        <v>#N/A Field Not Applicable</v>
+        <f t="array" ref="J3">IF(OR($C3="Corp", $C3="Govt"), IF($B3="TICKER", _xll.BDP($A3,J$1), _xll.BDP($A3&amp;" "&amp;$B3, J$1)), "#N/A")</f>
+        <v>#N/A</v>
       </c>
       <c r="K3" t="str" cm="1">
         <f t="array" ref="K3">IF(OR($C3="Corp", $C3="Govt"), IF($B3="TICKER", _xll.BDP($A3,K$1), _xll.BDP($A3&amp;" "&amp;$B3, K$1)), "#N/A")</f>
-        <v>BB+</v>
+        <v>#N/A</v>
       </c>
       <c r="L3" t="str" cm="1">
         <f t="array" ref="L3">IF(OR($C3="Corp", $C3="Govt"), IF($B3="TICKER", _xll.BDP($A3,L$1), _xll.BDP($A3&amp;" "&amp;$B3, L$1)), "#N/A")</f>
-        <v>Ba1</v>
-      </c>
-      <c r="M3" t="str" cm="1">
-        <f t="array" ref="M3">IF(OR($C3="Corp", $C3="Govt"), IF($B3="TICKER", _xll.BDP($A3,M$1), _xll.BDP($A3&amp;" "&amp;$B3, M$1)), "#N/A")</f>
-        <v>BBB</v>
+        <v>#N/A</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
@@ -882,47 +798,43 @@
       </c>
       <c r="C4" t="str" cm="1">
         <f t="array" ref="C4">IF($B4="TICKER", _xll.BDP($A4,C$1), _xll.BDP($A4&amp;" "&amp;$B4, C$1))</f>
-        <v>Corp</v>
+        <v>#N/A Connection</v>
       </c>
       <c r="D4" t="str" cm="1">
         <f t="array" ref="D4">IF($B4="TICKER", _xll.BDP($A4,D$1), _xll.BDP($A4&amp;" "&amp;$B4, D$1))</f>
-        <v>CN</v>
+        <v>#N/A Connection</v>
       </c>
       <c r="E4" t="str" cm="1">
         <f t="array" ref="E4">IF($B4="TICKER", _xll.BDP($A4,E$1), _xll.BDP($A4&amp;" "&amp;$B4, E$1))</f>
-        <v>CN</v>
+        <v>#N/A Connection</v>
       </c>
       <c r="F4" t="str" cm="1">
         <f t="array" ref="F4">IF($B4="TICKER", _xll.BDP($A4,F$1), _xll.BDP($A4&amp;" "&amp;$B4, F$1))</f>
-        <v>Corp</v>
+        <v>#N/A Connection</v>
       </c>
       <c r="G4" t="str" cm="1">
         <f t="array" ref="G4">IF($B4="TICKER", _xll.BDP($A4,G$1), _xll.BDP($A4&amp;" "&amp;$B4, G$1))</f>
-        <v>ACTV</v>
+        <v>#N/A Connection</v>
       </c>
       <c r="H4" t="str" cm="1">
-        <f t="array" ref="H4">IF($B4="TICKER", _xll.BDP($A4,H$1), _xll.BDP($A4&amp;" "&amp;$B4, H$1))</f>
-        <v>Financial</v>
+        <f t="array" ref="H4">IF(C4="Equity", "N", IF($B4="TICKER", _xll.BDP($A4,H$1), _xll.BDP($A4&amp;" "&amp;$B4, H$1)))</f>
+        <v>#N/A Connection</v>
       </c>
       <c r="I4" t="str" cm="1">
-        <f t="array" ref="I4">IF(C4="Equity", "N", IF($B4="TICKER", _xll.BDP($A4,I$1), _xll.BDP($A4&amp;" "&amp;$B4, I$1)))</f>
-        <v>Y</v>
+        <f t="array" ref="I4">IF($B4="TICKER", _xll.BDP($A4,I$1), _xll.BDP($A4&amp;" "&amp;$B4, I$1))</f>
+        <v>#N/A Connection</v>
       </c>
       <c r="J4" t="str" cm="1">
-        <f t="array" ref="J4">IF($B4="TICKER", _xll.BDP($A4,J$1), _xll.BDP($A4&amp;" "&amp;$B4, J$1))</f>
-        <v>#N/A Field Not Applicable</v>
+        <f t="array" ref="J4">IF(OR($C4="Corp", $C4="Govt"), IF($B4="TICKER", _xll.BDP($A4,J$1), _xll.BDP($A4&amp;" "&amp;$B4, J$1)), "#N/A")</f>
+        <v>#N/A</v>
       </c>
       <c r="K4" t="str" cm="1">
         <f t="array" ref="K4">IF(OR($C4="Corp", $C4="Govt"), IF($B4="TICKER", _xll.BDP($A4,K$1), _xll.BDP($A4&amp;" "&amp;$B4, K$1)), "#N/A")</f>
-        <v>BB+</v>
+        <v>#N/A</v>
       </c>
       <c r="L4" t="str" cm="1">
         <f t="array" ref="L4">IF(OR($C4="Corp", $C4="Govt"), IF($B4="TICKER", _xll.BDP($A4,L$1), _xll.BDP($A4&amp;" "&amp;$B4, L$1)), "#N/A")</f>
-        <v>Ba1</v>
-      </c>
-      <c r="M4" t="str" cm="1">
-        <f t="array" ref="M4">IF(OR($C4="Corp", $C4="Govt"), IF($B4="TICKER", _xll.BDP($A4,M$1), _xll.BDP($A4&amp;" "&amp;$B4, M$1)), "#N/A")</f>
-        <v>BB+</v>
+        <v>#N/A</v>
       </c>
     </row>
   </sheetData>

</xml_diff>